<commit_message>
change the experimentation results according to new formula
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="17850"/>
+    <workbookView windowWidth="20775" windowHeight="8505"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -13,8 +13,85 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>rcaldas</author>
+  </authors>
+  <commentList>
+    <comment ref="K13" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <rFont val="Times New Roman"/>
+            <charset val="0"/>
+          </rPr>
+          <t>rcaldas:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="Times New Roman"/>
+            <charset val="0"/>
+          </rPr>
+          <t xml:space="preserve">
+rcaldas:
+we expect that divine returns error found = yes, because it raises an error if enough accepting flags were raised. Indicating that the automata stayed in state 1 for long enough. This means that the system stabilized.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K14" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <rFont val="Times New Roman"/>
+            <charset val="0"/>
+          </rPr>
+          <t>rcaldas:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="Times New Roman"/>
+            <charset val="0"/>
+          </rPr>
+          <t xml:space="preserve">
+we expect that divine returns error found = yes, because it raises an error if enough accepting flags were raised. Indicating that the automata stayed in state 1 for long enough. This means that the system stabilized.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K15" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <rFont val="Times New Roman"/>
+            <charset val="0"/>
+          </rPr>
+          <t>rcaldas:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="Times New Roman"/>
+            <charset val="0"/>
+          </rPr>
+          <t xml:space="preserve">
+we expect that divine returns error found = no, because the automata will end up either in states 0 or 2. Indicating that the system was not eventually always in safe state.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="43">
   <si>
     <t>Towards Mapping CT and SE properties</t>
   </si>
@@ -31,7 +108,7 @@
     <t xml:space="preserve">Formula*: </t>
   </si>
   <si>
-    <t>[](!safe -&gt; &lt;&gt;([]safe))</t>
+    <t>&lt;&gt;([]safe)</t>
   </si>
   <si>
     <t>* The Büchi Automata was generated using Spot (https://spot.lrde.epita.fr/app/). Then,  the never claim was implemented by hand in the target code (next function in main.cpp).</t>
@@ -43,9 +120,6 @@
     <t>Complete</t>
   </si>
   <si>
-    <t>e_d = d_safe - d_rel</t>
-  </si>
-  <si>
     <t>ID</t>
   </si>
   <si>
@@ -115,10 +189,10 @@
     <t>0.1</t>
   </si>
   <si>
-    <t>e_d &lt;= 0</t>
-  </si>
-  <si>
-    <t>Success</t>
+    <t>d_rel - d_safe &gt; 0.05 * d_safe</t>
+  </si>
+  <si>
+    <t>Error found: yes</t>
   </si>
   <si>
     <t>my_mpcACCsystem.report.case1</t>
@@ -139,7 +213,7 @@
     <t>Case 3</t>
   </si>
   <si>
-    <t>Failure</t>
+    <t>Error found: no</t>
   </si>
   <si>
     <t>my_mpcACCsystem.report.case3</t>
@@ -158,7 +232,7 @@
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -169,44 +243,143 @@
     <font>
       <u/>
       <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
       <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -220,103 +393,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="9"/>
+      <name val="Times New Roman"/>
+      <charset val="0"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
+      <sz val="9"/>
+      <name val="Times New Roman"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="34">
@@ -346,175 +431,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -539,15 +624,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -582,26 +658,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -621,7 +677,36 @@
       <right/>
       <top/>
       <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -630,133 +715,133 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="7" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="3" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="2" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="2" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="3" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -765,13 +850,13 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -797,13 +882,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="true">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="48" applyBorder="true" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="48" applyAlignment="true">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="48" applyFont="true" applyBorder="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="48" applyFont="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="48" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="48" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1222,7 +1307,7 @@
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J18" sqref="J18"/>
+      <selection pane="bottomRight" activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.78" defaultRowHeight="15.75"/>
@@ -1288,17 +1373,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="10:10">
-      <c r="J10" t="s">
-        <v>9</v>
-      </c>
-    </row>
     <row r="11" spans="1:16">
       <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -1308,13 +1388,13 @@
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" t="s">
+        <v>11</v>
+      </c>
+      <c r="K11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="K11" s="2" t="s">
+      <c r="M11" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="M11" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
@@ -1322,63 +1402,63 @@
     </row>
     <row r="12" spans="1:16">
       <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" t="s">
         <v>15</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>16</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>17</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>18</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>19</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>20</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>21</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>22</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
         <v>23</v>
       </c>
-      <c r="J12" t="s">
+      <c r="K12" t="s">
         <v>24</v>
       </c>
-      <c r="K12" t="s">
+      <c r="L12" t="s">
         <v>25</v>
       </c>
-      <c r="L12" t="s">
+      <c r="M12" t="s">
         <v>26</v>
       </c>
-      <c r="M12" t="s">
+      <c r="N12" t="s">
         <v>27</v>
       </c>
-      <c r="N12" t="s">
+      <c r="O12" t="s">
         <v>28</v>
       </c>
-      <c r="O12" t="s">
+      <c r="P12" t="s">
         <v>29</v>
-      </c>
-      <c r="P12" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:16">
       <c r="A13" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B13" s="3">
         <v>35</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D13" s="3">
         <v>10</v>
@@ -1399,32 +1479,32 @@
         <v>1</v>
       </c>
       <c r="J13" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="K13" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="K13" s="4" t="s">
-        <v>34</v>
-      </c>
       <c r="L13" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M13" s="6"/>
       <c r="N13" s="3"/>
       <c r="O13" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="P13" s="8" t="s">
         <v>35</v>
-      </c>
-      <c r="P13" s="8" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:16">
       <c r="A14" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B14" s="3">
         <v>35</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D14" s="3">
         <v>20</v>
@@ -1445,32 +1525,32 @@
         <v>1</v>
       </c>
       <c r="J14" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="K14" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="K14" s="4" t="s">
-        <v>34</v>
-      </c>
       <c r="L14" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M14" s="6"/>
       <c r="N14" s="3"/>
-      <c r="O14" s="7" t="s">
+      <c r="O14" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="P14" s="7" t="s">
         <v>38</v>
-      </c>
-      <c r="P14" s="9" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:16">
       <c r="A15" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B15" s="3">
         <v>35</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D15" s="3">
         <v>40</v>
@@ -1491,21 +1571,21 @@
         <v>1</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L15" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M15" s="6"/>
       <c r="N15" s="3"/>
-      <c r="O15" s="7" t="s">
+      <c r="O15" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="P15" s="7" t="s">
         <v>42</v>
-      </c>
-      <c r="P15" s="9" t="s">
-        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1515,17 +1595,18 @@
     <mergeCell ref="M11:P11"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="P14" r:id="rId2" display="case2.png"/>
-    <hyperlink ref="P15" r:id="rId3" display="case3.png"/>
-    <hyperlink ref="O13" r:id="rId4" display="my_mpcACCsystem.report.case1"/>
-    <hyperlink ref="O14" r:id="rId5" display="my_mpcACCsystem.report.case2"/>
-    <hyperlink ref="O15" r:id="rId6" display="my_mpcACCsystem.report.case3"/>
-    <hyperlink ref="P13" r:id="rId7" display="case1.png"/>
+    <hyperlink ref="P14" r:id="rId4" display="case2.png"/>
+    <hyperlink ref="P15" r:id="rId5" display="case3.png"/>
+    <hyperlink ref="O13" r:id="rId6" display="my_mpcACCsystem.report.case1"/>
+    <hyperlink ref="O14" r:id="rId7" display="my_mpcACCsystem.report.case2"/>
+    <hyperlink ref="O15" r:id="rId8" display="my_mpcACCsystem.report.case3"/>
+    <hyperlink ref="P13" r:id="rId9" display="case1.png"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
+  <legacyDrawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>